<commit_message>
configured support email and added tax sugesstions in Chatbot
</commit_message>
<xml_diff>
--- a/data/NVDA_financial_data.xlsx
+++ b/data/NVDA_financial_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t>Tax Effect Of Unusual Items</t>
   </si>
@@ -285,9 +285,6 @@
     <t>Payables</t>
   </si>
   <si>
-    <t>Other Payable</t>
-  </si>
-  <si>
     <t>Total Tax Payable</t>
   </si>
   <si>
@@ -312,12 +309,21 @@
     <t>Non Current Deferred Taxes Assets</t>
   </si>
   <si>
+    <t>Non Current Accounts Receivable</t>
+  </si>
+  <si>
     <t>Investments And Advances</t>
   </si>
   <si>
     <t>Other Investments</t>
   </si>
   <si>
+    <t>Investmentin Financial Assets</t>
+  </si>
+  <si>
+    <t>Available For Sale Securities</t>
+  </si>
+  <si>
     <t>Goodwill And Other Intangible Assets</t>
   </si>
   <si>
@@ -471,6 +477,9 @@
     <t>Cash Flow From Continuing Investing Activities</t>
   </si>
   <si>
+    <t>Net Other Investing Changes</t>
+  </si>
+  <si>
     <t>Net Investment Purchase And Sale</t>
   </si>
   <si>
@@ -489,9 +498,6 @@
     <t>Net PPE Purchase And Sale</t>
   </si>
   <si>
-    <t>Sale Of PPE</t>
-  </si>
-  <si>
     <t>Purchase Of PPE</t>
   </si>
   <si>
@@ -553,6 +559,15 @@
   </si>
   <si>
     <t>Depreciation And Amortization</t>
+  </si>
+  <si>
+    <t>Amortization Cash Flow</t>
+  </si>
+  <si>
+    <t>Amortization Of Intangibles</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
   </si>
   <si>
     <t>Operating Gains Losses</t>
@@ -933,16 +948,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1">
+        <v>45688</v>
+      </c>
+      <c r="C1" s="1">
         <v>45322</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>44957</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>44592</v>
-      </c>
-      <c r="E1" s="1">
-        <v>44227</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -953,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>-284130000</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -967,16 +982,16 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>0.133</v>
+      </c>
+      <c r="C3">
         <v>0.12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.21</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.019</v>
-      </c>
-      <c r="E3">
-        <v>0.017</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -984,16 +999,16 @@
         <v>2</v>
       </c>
       <c r="B4">
+        <v>86137000000</v>
+      </c>
+      <c r="C4">
         <v>35583000000</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>7340000000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>11351000000</v>
-      </c>
-      <c r="E4">
-        <v>5691000000</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1004,10 +1019,10 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>-1353000000</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1021,10 +1036,10 @@
         <v>0</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>-1353000000</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1035,16 +1050,16 @@
         <v>5</v>
       </c>
       <c r="B7">
+        <v>72880000000</v>
+      </c>
+      <c r="C7">
         <v>29760000000</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>4368000000</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>9752000000</v>
-      </c>
-      <c r="E7">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1052,16 +1067,16 @@
         <v>6</v>
       </c>
       <c r="B8">
+        <v>1864000000</v>
+      </c>
+      <c r="C8">
         <v>1508000000</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1544000000</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1174000000</v>
-      </c>
-      <c r="E8">
-        <v>1098000000</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1069,16 +1084,16 @@
         <v>7</v>
       </c>
       <c r="B9">
+        <v>32639000000</v>
+      </c>
+      <c r="C9">
         <v>16621000000</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>11618000000</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>9439000000</v>
-      </c>
-      <c r="E9">
-        <v>6279000000</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1086,16 +1101,16 @@
         <v>8</v>
       </c>
       <c r="B10">
+        <v>86137000000</v>
+      </c>
+      <c r="C10">
         <v>35583000000</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>5987000000</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>11351000000</v>
-      </c>
-      <c r="E10">
-        <v>5691000000</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1103,16 +1118,16 @@
         <v>9</v>
       </c>
       <c r="B11">
+        <v>84273000000</v>
+      </c>
+      <c r="C11">
         <v>34075000000</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>4443000000</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>10177000000</v>
-      </c>
-      <c r="E11">
-        <v>4593000000</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1120,16 +1135,16 @@
         <v>10</v>
       </c>
       <c r="B12">
+        <v>1539000000</v>
+      </c>
+      <c r="C12">
         <v>609000000</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>5000000</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>-207000000</v>
-      </c>
-      <c r="E12">
-        <v>-127000000</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1137,16 +1152,16 @@
         <v>11</v>
       </c>
       <c r="B13">
+        <v>247000000</v>
+      </c>
+      <c r="C13">
         <v>257000000</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>262000000</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>236000000</v>
-      </c>
-      <c r="E13">
-        <v>184000000</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1154,16 +1169,16 @@
         <v>12</v>
       </c>
       <c r="B14">
+        <v>1786000000</v>
+      </c>
+      <c r="C14">
         <v>866000000</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>267000000</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>29000000</v>
-      </c>
-      <c r="E14">
-        <v>57000000</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1171,16 +1186,16 @@
         <v>13</v>
       </c>
       <c r="B15">
+        <v>72880000000</v>
+      </c>
+      <c r="C15">
         <v>29760000000</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>5436870000</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>9752000000</v>
-      </c>
-      <c r="E15">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1188,16 +1203,16 @@
         <v>14</v>
       </c>
       <c r="B16">
+        <v>72880000000</v>
+      </c>
+      <c r="C16">
         <v>29760000000</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>4368000000</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>9752000000</v>
-      </c>
-      <c r="E16">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1205,16 +1220,16 @@
         <v>15</v>
       </c>
       <c r="B17">
+        <v>49044000000</v>
+      </c>
+      <c r="C17">
         <v>27950000000</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>21397000000</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>16873000000</v>
-      </c>
-      <c r="E17">
-        <v>12143000000</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1222,16 +1237,16 @@
         <v>16</v>
       </c>
       <c r="B18">
+        <v>81453000000</v>
+      </c>
+      <c r="C18">
         <v>32972000000</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>4224000000</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>10041000000</v>
-      </c>
-      <c r="E18">
-        <v>4532000000</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1239,16 +1254,16 @@
         <v>17</v>
       </c>
       <c r="B19">
+        <v>24804000000</v>
+      </c>
+      <c r="C19">
         <v>24940000000</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>25070000000</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>25350000000</v>
-      </c>
-      <c r="E19">
-        <v>25120000000</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1256,16 +1271,16 @@
         <v>18</v>
       </c>
       <c r="B20">
+        <v>24555000000</v>
+      </c>
+      <c r="C20">
         <v>24690000000</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>24870000000</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>24960000000</v>
-      </c>
-      <c r="E20">
-        <v>24680000000</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1273,16 +1288,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1.193</v>
+        <v>2.94</v>
       </c>
       <c r="C21">
-        <v>0.174</v>
+        <v>1.19</v>
       </c>
       <c r="D21">
+        <v>0.17</v>
+      </c>
+      <c r="E21">
         <v>0.385</v>
-      </c>
-      <c r="E21">
-        <v>0.1725</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1290,16 +1305,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.205</v>
+        <v>2.97</v>
       </c>
       <c r="C22">
-        <v>0.176</v>
+        <v>1.21</v>
       </c>
       <c r="D22">
+        <v>0.18</v>
+      </c>
+      <c r="E22">
         <v>0.391</v>
-      </c>
-      <c r="E22">
-        <v>0.1755</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1307,16 +1322,16 @@
         <v>21</v>
       </c>
       <c r="B23">
+        <v>72880000000</v>
+      </c>
+      <c r="C23">
         <v>29760000000</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>4368000000</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>9752000000</v>
-      </c>
-      <c r="E23">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1324,16 +1339,16 @@
         <v>22</v>
       </c>
       <c r="B24">
+        <v>72880000000</v>
+      </c>
+      <c r="C24">
         <v>29760000000</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>4368000000</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>9752000000</v>
-      </c>
-      <c r="E24">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1341,16 +1356,16 @@
         <v>23</v>
       </c>
       <c r="B25">
+        <v>72880000000</v>
+      </c>
+      <c r="C25">
         <v>29760000000</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>4368000000</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>9752000000</v>
-      </c>
-      <c r="E25">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1358,16 +1373,16 @@
         <v>24</v>
       </c>
       <c r="B26">
+        <v>72880000000</v>
+      </c>
+      <c r="C26">
         <v>29760000000</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>4368000000</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>9752000000</v>
-      </c>
-      <c r="E26">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1375,16 +1390,16 @@
         <v>25</v>
       </c>
       <c r="B27">
+        <v>72880000000</v>
+      </c>
+      <c r="C27">
         <v>29760000000</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>4368000000</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>9752000000</v>
-      </c>
-      <c r="E27">
-        <v>4332000000</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1392,16 +1407,16 @@
         <v>26</v>
       </c>
       <c r="B28">
+        <v>11146000000</v>
+      </c>
+      <c r="C28">
         <v>4058000000</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>-187000000</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>189000000</v>
-      </c>
-      <c r="E28">
-        <v>77000000</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1409,16 +1424,16 @@
         <v>27</v>
       </c>
       <c r="B29">
+        <v>84026000000</v>
+      </c>
+      <c r="C29">
         <v>33818000000</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>4181000000</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>9941000000</v>
-      </c>
-      <c r="E29">
-        <v>4409000000</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1426,16 +1441,16 @@
         <v>28</v>
       </c>
       <c r="B30">
+        <v>1034000000</v>
+      </c>
+      <c r="C30">
         <v>237000000</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>-1401000000</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>107000000</v>
-      </c>
-      <c r="E30">
-        <v>4000000</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1443,16 +1458,16 @@
         <v>29</v>
       </c>
       <c r="B31">
+        <v>1034000000</v>
+      </c>
+      <c r="C31">
         <v>237000000</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>-48000000</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>107000000</v>
-      </c>
-      <c r="E31">
-        <v>4000000</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1463,10 +1478,10 @@
         <v>0</v>
       </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>-1353000000</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1480,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>1353000000</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1494,16 +1509,16 @@
         <v>32</v>
       </c>
       <c r="B34">
+        <v>1539000000</v>
+      </c>
+      <c r="C34">
         <v>609000000</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>5000000</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>-207000000</v>
-      </c>
-      <c r="E34">
-        <v>-127000000</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1511,16 +1526,16 @@
         <v>33</v>
       </c>
       <c r="B35">
+        <v>247000000</v>
+      </c>
+      <c r="C35">
         <v>257000000</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>262000000</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>236000000</v>
-      </c>
-      <c r="E35">
-        <v>184000000</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1528,16 +1543,16 @@
         <v>34</v>
       </c>
       <c r="B36">
+        <v>1786000000</v>
+      </c>
+      <c r="C36">
         <v>866000000</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>267000000</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>29000000</v>
-      </c>
-      <c r="E36">
-        <v>57000000</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1545,16 +1560,16 @@
         <v>35</v>
       </c>
       <c r="B37">
+        <v>81453000000</v>
+      </c>
+      <c r="C37">
         <v>32972000000</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>5577000000</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>10041000000</v>
-      </c>
-      <c r="E37">
-        <v>4532000000</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1562,16 +1577,16 @@
         <v>36</v>
       </c>
       <c r="B38">
+        <v>16405000000</v>
+      </c>
+      <c r="C38">
         <v>11329000000</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>9779000000</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>7434000000</v>
-      </c>
-      <c r="E38">
-        <v>5864000000</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1579,16 +1594,16 @@
         <v>37</v>
       </c>
       <c r="B39">
+        <v>12914000000</v>
+      </c>
+      <c r="C39">
         <v>8675000000</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>7339000000</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>5268000000</v>
-      </c>
-      <c r="E39">
-        <v>3924000000</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1596,16 +1611,16 @@
         <v>38</v>
       </c>
       <c r="B40">
+        <v>3491000000</v>
+      </c>
+      <c r="C40">
         <v>2654000000</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>2440000000</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>2166000000</v>
-      </c>
-      <c r="E40">
-        <v>1940000000</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1613,16 +1628,16 @@
         <v>39</v>
       </c>
       <c r="B41">
+        <v>97858000000</v>
+      </c>
+      <c r="C41">
         <v>44301000000</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>15356000000</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>17475000000</v>
-      </c>
-      <c r="E41">
-        <v>10396000000</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1630,16 +1645,16 @@
         <v>40</v>
       </c>
       <c r="B42">
+        <v>32639000000</v>
+      </c>
+      <c r="C42">
         <v>16621000000</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>11618000000</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>9439000000</v>
-      </c>
-      <c r="E42">
-        <v>6279000000</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1647,16 +1662,16 @@
         <v>41</v>
       </c>
       <c r="B43">
+        <v>130497000000</v>
+      </c>
+      <c r="C43">
         <v>60922000000</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>26974000000</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>26914000000</v>
-      </c>
-      <c r="E43">
-        <v>16675000000</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1664,16 +1679,16 @@
         <v>42</v>
       </c>
       <c r="B44">
+        <v>130497000000</v>
+      </c>
+      <c r="C44">
         <v>60922000000</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>26974000000</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>26914000000</v>
-      </c>
-      <c r="E44">
-        <v>16675000000</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +1698,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1691,30 +1706,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1">
+        <v>45688</v>
+      </c>
+      <c r="C1" s="1">
         <v>45322</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>44957</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>44592</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>44227</v>
-      </c>
-      <c r="F1" s="1">
-        <v>43861</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>13800000000</v>
-      </c>
-      <c r="F2">
-        <v>13700576960</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1722,16 +1734,16 @@
         <v>44</v>
       </c>
       <c r="B3">
+        <v>24477000000</v>
+      </c>
+      <c r="C3">
         <v>24640000000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>24661365720</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>25060000000</v>
-      </c>
-      <c r="E3">
-        <v>24800000000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1739,32 +1751,32 @@
         <v>45</v>
       </c>
       <c r="B4">
+        <v>24477000000</v>
+      </c>
+      <c r="C4">
         <v>24640000000</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>24661365720</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>25060000000</v>
-      </c>
-      <c r="E4">
-        <v>38600000000</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2429000000</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>7564000000</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>8956000000</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6116000000</v>
       </c>
     </row>
@@ -1773,16 +1785,16 @@
         <v>47</v>
       </c>
       <c r="B6">
+        <v>10270000000</v>
+      </c>
+      <c r="C6">
         <v>11056000000</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>12031000000</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>11831000000</v>
-      </c>
-      <c r="E6">
-        <v>7597000000</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1790,16 +1802,16 @@
         <v>48</v>
       </c>
       <c r="B7">
+        <v>73332000000</v>
+      </c>
+      <c r="C7">
         <v>37436000000</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>16053000000</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>19924000000</v>
-      </c>
-      <c r="E7">
-        <v>9963000000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1807,16 +1819,16 @@
         <v>49</v>
       </c>
       <c r="B8">
+        <v>87790000000</v>
+      </c>
+      <c r="C8">
         <v>52687000000</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>33054000000</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>37558000000</v>
-      </c>
-      <c r="E8">
-        <v>23856000000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1824,16 +1836,16 @@
         <v>50</v>
       </c>
       <c r="B9">
+        <v>62079000000</v>
+      </c>
+      <c r="C9">
         <v>33714000000</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>16510000000</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>24494000000</v>
-      </c>
-      <c r="E9">
-        <v>12130000000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1841,16 +1853,16 @@
         <v>51</v>
       </c>
       <c r="B10">
+        <v>73332000000</v>
+      </c>
+      <c r="C10">
         <v>37436000000</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>16053000000</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>19924000000</v>
-      </c>
-      <c r="E10">
-        <v>9963000000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1858,16 +1870,16 @@
         <v>52</v>
       </c>
       <c r="B11">
+        <v>1807000000</v>
+      </c>
+      <c r="C11">
         <v>1347000000</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1078000000</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>885000000</v>
-      </c>
-      <c r="E11">
-        <v>634000000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1875,16 +1887,16 @@
         <v>53</v>
       </c>
       <c r="B12">
+        <v>79327000000</v>
+      </c>
+      <c r="C12">
         <v>42978000000</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>22101000000</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>26612000000</v>
-      </c>
-      <c r="E12">
-        <v>16893000000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1892,16 +1904,16 @@
         <v>54</v>
       </c>
       <c r="B13">
+        <v>87790000000</v>
+      </c>
+      <c r="C13">
         <v>51437000000</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>31804000000</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>37558000000</v>
-      </c>
-      <c r="E13">
-        <v>22857000000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1909,16 +1921,16 @@
         <v>55</v>
       </c>
       <c r="B14">
+        <v>79327000000</v>
+      </c>
+      <c r="C14">
         <v>42978000000</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>22101000000</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>26612000000</v>
-      </c>
-      <c r="E14">
-        <v>16893000000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1926,16 +1938,16 @@
         <v>56</v>
       </c>
       <c r="B15">
+        <v>79327000000</v>
+      </c>
+      <c r="C15">
         <v>42978000000</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>22101000000</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>26612000000</v>
-      </c>
-      <c r="E15">
-        <v>16893000000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1943,16 +1955,16 @@
         <v>57</v>
       </c>
       <c r="B16">
+        <v>28000000</v>
+      </c>
+      <c r="C16">
         <v>27000000</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>-43000000</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>-11000000</v>
-      </c>
-      <c r="E16">
-        <v>19000000</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1960,30 +1972,27 @@
         <v>58</v>
       </c>
       <c r="B17">
+        <v>28000000</v>
+      </c>
+      <c r="C17">
         <v>27000000</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>-43000000</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-11000000</v>
-      </c>
-      <c r="E17">
-        <v>19000000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>10756000000</v>
-      </c>
-      <c r="F18">
-        <v>9814000000</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1991,16 +2000,16 @@
         <v>60</v>
       </c>
       <c r="B19">
+        <v>68038000000</v>
+      </c>
+      <c r="C19">
         <v>29817000000</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>10171000000</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>16235000000</v>
-      </c>
-      <c r="E19">
-        <v>18908000000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2008,16 +2017,16 @@
         <v>61</v>
       </c>
       <c r="B20">
-        <v>13132000000</v>
+        <v>11237000000</v>
       </c>
       <c r="C20">
+        <v>13109000000</v>
+      </c>
+      <c r="D20">
         <v>11971000000</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>10385000000</v>
-      </c>
-      <c r="E20">
-        <v>8719000000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2025,13 +2034,13 @@
         <v>62</v>
       </c>
       <c r="B21">
+        <v>24000000</v>
+      </c>
+      <c r="C21">
+        <v>25000000</v>
+      </c>
+      <c r="D21">
         <v>2000000</v>
-      </c>
-      <c r="C21">
-        <v>2000000</v>
-      </c>
-      <c r="D21">
-        <v>3000000</v>
       </c>
       <c r="E21">
         <v>3000000</v>
@@ -2042,13 +2051,13 @@
         <v>63</v>
       </c>
       <c r="B22">
+        <v>24000000</v>
+      </c>
+      <c r="C22">
+        <v>25000000</v>
+      </c>
+      <c r="D22">
         <v>2000000</v>
-      </c>
-      <c r="C22">
-        <v>2000000</v>
-      </c>
-      <c r="D22">
-        <v>3000000</v>
       </c>
       <c r="E22">
         <v>3000000</v>
@@ -2076,16 +2085,16 @@
         <v>65</v>
       </c>
       <c r="B24">
+        <v>32274000000</v>
+      </c>
+      <c r="C24">
         <v>22750000000</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>19081000000</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>17575000000</v>
-      </c>
-      <c r="E24">
-        <v>11898000000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2093,16 +2102,16 @@
         <v>66</v>
       </c>
       <c r="B25">
+        <v>14227000000</v>
+      </c>
+      <c r="C25">
         <v>12119000000</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>12518000000</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>13240000000</v>
-      </c>
-      <c r="E25">
-        <v>7973000000</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2110,27 +2119,24 @@
         <v>67</v>
       </c>
       <c r="B26">
+        <v>79000000</v>
+      </c>
+      <c r="C26">
         <v>65000000</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>63000000</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>49000000</v>
-      </c>
-      <c r="E26">
-        <v>135000000</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>33000000</v>
-      </c>
-      <c r="F27">
-        <v>22000000</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2138,16 +2144,16 @@
         <v>69</v>
       </c>
       <c r="B28">
+        <v>2304000000</v>
+      </c>
+      <c r="C28">
         <v>1441000000</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>1385000000</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>1057000000</v>
-      </c>
-      <c r="E28">
-        <v>836000000</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2155,16 +2161,16 @@
         <v>70</v>
       </c>
       <c r="B29">
+        <v>1862000000</v>
+      </c>
+      <c r="C29">
         <v>1035000000</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>465000000</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>447000000</v>
-      </c>
-      <c r="E29">
-        <v>404000000</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2172,16 +2178,16 @@
         <v>71</v>
       </c>
       <c r="B30">
+        <v>976000000</v>
+      </c>
+      <c r="C30">
         <v>573000000</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>218000000</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>202000000</v>
-      </c>
-      <c r="E30">
-        <v>163000000</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2189,16 +2195,16 @@
         <v>72</v>
       </c>
       <c r="B31">
+        <v>886000000</v>
+      </c>
+      <c r="C31">
         <v>462000000</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>247000000</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>245000000</v>
-      </c>
-      <c r="E31">
-        <v>241000000</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2206,16 +2212,16 @@
         <v>73</v>
       </c>
       <c r="B32">
+        <v>9982000000</v>
+      </c>
+      <c r="C32">
         <v>9578000000</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>10605000000</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>11687000000</v>
-      </c>
-      <c r="E32">
-        <v>6598000000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2223,16 +2229,16 @@
         <v>74</v>
       </c>
       <c r="B33">
+        <v>1519000000</v>
+      </c>
+      <c r="C33">
         <v>1119000000</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>902000000</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>741000000</v>
-      </c>
-      <c r="E33">
-        <v>634000000</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2240,16 +2246,16 @@
         <v>75</v>
       </c>
       <c r="B34">
+        <v>8463000000</v>
+      </c>
+      <c r="C34">
         <v>8459000000</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>9703000000</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>10946000000</v>
-      </c>
-      <c r="E34">
-        <v>5964000000</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2257,16 +2263,16 @@
         <v>76</v>
       </c>
       <c r="B35">
+        <v>18047000000</v>
+      </c>
+      <c r="C35">
         <v>10631000000</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>6563000000</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>4335000000</v>
-      </c>
-      <c r="E35">
-        <v>3925000000</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2274,16 +2280,16 @@
         <v>77</v>
       </c>
       <c r="B36">
+        <v>228000000</v>
+      </c>
+      <c r="C36">
         <v>199000000</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>69000000</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>371000000</v>
-      </c>
-      <c r="E36">
-        <v>510000000</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2291,16 +2297,16 @@
         <v>78</v>
       </c>
       <c r="B37">
+        <v>837000000</v>
+      </c>
+      <c r="C37">
         <v>764000000</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>354000000</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>300000000</v>
-      </c>
-      <c r="E37">
-        <v>288000000</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2308,16 +2314,16 @@
         <v>79</v>
       </c>
       <c r="B38">
+        <v>837000000</v>
+      </c>
+      <c r="C38">
         <v>764000000</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>354000000</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>300000000</v>
-      </c>
-      <c r="E38">
-        <v>288000000</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2325,16 +2331,16 @@
         <v>80</v>
       </c>
       <c r="B39">
+        <v>288000000</v>
+      </c>
+      <c r="C39">
         <v>1478000000</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>1426000000</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>144000000</v>
-      </c>
-      <c r="E39">
-        <v>999000000</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2342,29 +2348,29 @@
         <v>81</v>
       </c>
       <c r="B40">
+        <v>288000000</v>
+      </c>
+      <c r="C40">
         <v>228000000</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>176000000</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>144000000</v>
-      </c>
-      <c r="E40">
-        <v>121000000</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B41">
-        <v>1250000000</v>
-      </c>
       <c r="C41">
         <v>1250000000</v>
       </c>
-      <c r="E41">
+      <c r="D41">
+        <v>1250000000</v>
+      </c>
+      <c r="F41">
         <v>999000000</v>
       </c>
     </row>
@@ -2372,13 +2378,13 @@
       <c r="A42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B42">
-        <v>1250000000</v>
-      </c>
       <c r="C42">
         <v>1250000000</v>
       </c>
-      <c r="E42">
+      <c r="D42">
+        <v>1250000000</v>
+      </c>
+      <c r="F42">
         <v>999000000</v>
       </c>
     </row>
@@ -2387,9 +2393,12 @@
         <v>84</v>
       </c>
       <c r="B43">
+        <v>1373000000</v>
+      </c>
+      <c r="C43">
         <v>415000000</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>108000000</v>
       </c>
     </row>
@@ -2398,16 +2407,16 @@
         <v>85</v>
       </c>
       <c r="B44">
+        <v>15321000000</v>
+      </c>
+      <c r="C44">
         <v>7775000000</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>4606000000</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>3520000000</v>
-      </c>
-      <c r="E44">
-        <v>2128000000</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2415,27 +2424,24 @@
         <v>86</v>
       </c>
       <c r="B45">
+        <v>8130000000</v>
+      </c>
+      <c r="C45">
         <v>4780000000</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>2946000000</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>1605000000</v>
-      </c>
-      <c r="E45">
-        <v>979000000</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>74000000</v>
-      </c>
-      <c r="F46">
-        <v>20000000</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2443,307 +2449,301 @@
         <v>88</v>
       </c>
       <c r="B47">
+        <v>7191000000</v>
+      </c>
+      <c r="C47">
         <v>2995000000</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>1660000000</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>1915000000</v>
-      </c>
-      <c r="E47">
-        <v>1149000000</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F48">
-        <v>54000000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="B48">
+        <v>881000000</v>
+      </c>
+      <c r="C48">
+        <v>296000000</v>
+      </c>
+      <c r="D48">
+        <v>467000000</v>
+      </c>
+      <c r="E48">
+        <v>132000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B49">
-        <v>296000000</v>
+        <v>6310000000</v>
       </c>
       <c r="C49">
-        <v>467000000</v>
+        <v>2699000000</v>
       </c>
       <c r="D49">
-        <v>132000000</v>
+        <v>1193000000</v>
       </c>
       <c r="E49">
-        <v>61000000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>1783000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B50">
-        <v>2699000000</v>
+        <v>111601000000</v>
       </c>
       <c r="C50">
-        <v>1193000000</v>
+        <v>65728000000</v>
       </c>
       <c r="D50">
-        <v>1783000000</v>
+        <v>41182000000</v>
       </c>
       <c r="E50">
-        <v>1149000000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>44187000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B51">
-        <v>65728000000</v>
+        <v>31475000000</v>
       </c>
       <c r="C51">
-        <v>41182000000</v>
+        <v>21383000000</v>
       </c>
       <c r="D51">
-        <v>44187000000</v>
+        <v>18109000000</v>
       </c>
       <c r="E51">
-        <v>28791000000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>15358000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B52">
-        <v>21383000000</v>
+        <v>201000000</v>
       </c>
       <c r="C52">
-        <v>18109000000</v>
+        <v>357000000</v>
       </c>
       <c r="D52">
-        <v>15358000000</v>
+        <v>145000000</v>
       </c>
       <c r="E52">
-        <v>12736000000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>66000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B53">
-        <v>132000000</v>
+        <v>2087000000</v>
       </c>
       <c r="C53">
-        <v>145000000</v>
+        <v>2822000000</v>
       </c>
       <c r="D53">
-        <v>66000000</v>
+        <v>3376000000</v>
       </c>
       <c r="E53">
-        <v>203000000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>3509000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B54">
-        <v>2822000000</v>
+        <v>10979000000</v>
       </c>
       <c r="C54">
-        <v>3376000000</v>
+        <v>6081000000</v>
       </c>
       <c r="D54">
-        <v>3509000000</v>
+        <v>3396000000</v>
       </c>
       <c r="E54">
-        <v>1797000000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>1222000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B55">
+        <v>10979000000</v>
+      </c>
+      <c r="C55">
         <v>6081000000</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>3396000000</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>1222000000</v>
       </c>
-      <c r="E55">
-        <v>806000000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B56">
-        <v>6081000000</v>
-      </c>
-      <c r="C56">
-        <v>3396000000</v>
-      </c>
-      <c r="D56">
-        <v>1222000000</v>
-      </c>
-      <c r="E56">
-        <v>806000000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>750000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B57">
-        <v>1546000000</v>
+        <v>3387000000</v>
       </c>
       <c r="C57">
+        <v>1321000000</v>
+      </c>
+      <c r="D57">
         <v>299000000</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>266000000</v>
       </c>
-      <c r="E57">
-        <v>144000000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>1546000000</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>299000000</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>266000000</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>144000000</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B59">
-        <v>5542000000</v>
+        <v>3387000000</v>
       </c>
       <c r="C59">
-        <v>6048000000</v>
-      </c>
-      <c r="D59">
-        <v>6688000000</v>
-      </c>
-      <c r="E59">
-        <v>6930000000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>1321000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B60">
-        <v>1112000000</v>
+        <v>3387000000</v>
       </c>
       <c r="C60">
-        <v>1676000000</v>
-      </c>
-      <c r="D60">
-        <v>2339000000</v>
-      </c>
-      <c r="E60">
-        <v>2737000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>1321000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B61">
-        <v>4430000000</v>
+        <v>5995000000</v>
       </c>
       <c r="C61">
-        <v>4372000000</v>
+        <v>5542000000</v>
       </c>
       <c r="D61">
-        <v>4349000000</v>
+        <v>6048000000</v>
       </c>
       <c r="E61">
-        <v>4193000000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>6688000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B62">
-        <v>5260000000</v>
+        <v>807000000</v>
       </c>
       <c r="C62">
-        <v>4845000000</v>
+        <v>1112000000</v>
       </c>
       <c r="D62">
-        <v>3607000000</v>
+        <v>1676000000</v>
       </c>
       <c r="E62">
-        <v>2856000000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>2339000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B63">
-        <v>-3509000000</v>
+        <v>5188000000</v>
       </c>
       <c r="C63">
-        <v>-2694000000</v>
+        <v>4430000000</v>
       </c>
       <c r="D63">
-        <v>-1903000000</v>
+        <v>4372000000</v>
       </c>
       <c r="E63">
-        <v>-1408000000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>4349000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B64">
-        <v>8769000000</v>
+        <v>8076000000</v>
       </c>
       <c r="C64">
-        <v>7539000000</v>
+        <v>5260000000</v>
       </c>
       <c r="D64">
-        <v>5510000000</v>
+        <v>4845000000</v>
       </c>
       <c r="E64">
-        <v>4264000000</v>
+        <v>3607000000</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="B65">
+        <v>-4401000000</v>
+      </c>
+      <c r="C65">
+        <v>-3509000000</v>
+      </c>
+      <c r="D65">
+        <v>-2694000000</v>
+      </c>
       <c r="E65">
-        <v>385000000</v>
-      </c>
-      <c r="F65">
-        <v>293000000</v>
+        <v>-1903000000</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2751,33 +2751,24 @@
         <v>107</v>
       </c>
       <c r="B66">
-        <v>189000000</v>
+        <v>12477000000</v>
       </c>
       <c r="C66">
-        <v>382000000</v>
+        <v>8769000000</v>
       </c>
       <c r="D66">
-        <v>737000000</v>
+        <v>7539000000</v>
       </c>
       <c r="E66">
-        <v>558000000</v>
+        <v>5510000000</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B67">
-        <v>1346000000</v>
-      </c>
-      <c r="C67">
-        <v>1038000000</v>
-      </c>
-      <c r="D67">
-        <v>829000000</v>
-      </c>
-      <c r="E67">
-        <v>707000000</v>
+      <c r="F67">
+        <v>385000000</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2785,16 +2776,16 @@
         <v>109</v>
       </c>
       <c r="B68">
-        <v>5200000000</v>
+        <v>529000000</v>
       </c>
       <c r="C68">
-        <v>4303000000</v>
+        <v>189000000</v>
       </c>
       <c r="D68">
-        <v>2852000000</v>
+        <v>382000000</v>
       </c>
       <c r="E68">
-        <v>1985000000</v>
+        <v>737000000</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2802,16 +2793,16 @@
         <v>110</v>
       </c>
       <c r="B69">
-        <v>1816000000</v>
+        <v>1793000000</v>
       </c>
       <c r="C69">
-        <v>1598000000</v>
+        <v>1346000000</v>
       </c>
       <c r="D69">
-        <v>874000000</v>
+        <v>1038000000</v>
       </c>
       <c r="E69">
-        <v>796000000</v>
+        <v>829000000</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2819,16 +2810,16 @@
         <v>111</v>
       </c>
       <c r="B70">
-        <v>218000000</v>
+        <v>7568000000</v>
       </c>
       <c r="C70">
-        <v>218000000</v>
+        <v>5200000000</v>
       </c>
       <c r="D70">
-        <v>218000000</v>
+        <v>4303000000</v>
       </c>
       <c r="E70">
-        <v>218000000</v>
+        <v>2852000000</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2836,16 +2827,16 @@
         <v>112</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>2076000000</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1816000000</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1598000000</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>874000000</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2853,16 +2844,16 @@
         <v>113</v>
       </c>
       <c r="B72">
-        <v>44345000000</v>
+        <v>511000000</v>
       </c>
       <c r="C72">
-        <v>23073000000</v>
+        <v>218000000</v>
       </c>
       <c r="D72">
-        <v>28829000000</v>
+        <v>218000000</v>
       </c>
       <c r="E72">
-        <v>16055000000</v>
+        <v>218000000</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2870,30 +2861,33 @@
         <v>114</v>
       </c>
       <c r="B73">
-        <v>3080000000</v>
+        <v>0</v>
       </c>
       <c r="C73">
-        <v>791000000</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>366000000</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>239000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
         <v>115</v>
       </c>
+      <c r="B74">
+        <v>80126000000</v>
+      </c>
+      <c r="C74">
+        <v>44345000000</v>
+      </c>
       <c r="D74">
-        <v>366000000</v>
+        <v>23073000000</v>
       </c>
       <c r="E74">
-        <v>239000000</v>
-      </c>
-      <c r="F74">
-        <v>157000000</v>
+        <v>28829000000</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2901,33 +2895,27 @@
         <v>116</v>
       </c>
       <c r="B75">
-        <v>5282000000</v>
+        <v>3771000000</v>
       </c>
       <c r="C75">
-        <v>5159000000</v>
+        <v>3080000000</v>
       </c>
       <c r="D75">
-        <v>2605000000</v>
+        <v>791000000</v>
       </c>
       <c r="E75">
-        <v>1826000000</v>
+        <v>366000000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B76">
-        <v>2058000000</v>
-      </c>
-      <c r="C76">
-        <v>2263000000</v>
-      </c>
-      <c r="D76">
-        <v>1122000000</v>
-      </c>
       <c r="E76">
-        <v>737000000</v>
+        <v>366000000</v>
+      </c>
+      <c r="F76">
+        <v>239000000</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2935,16 +2923,16 @@
         <v>118</v>
       </c>
       <c r="B77">
-        <v>1505000000</v>
+        <v>10080000000</v>
       </c>
       <c r="C77">
-        <v>466000000</v>
+        <v>5282000000</v>
       </c>
       <c r="D77">
-        <v>692000000</v>
+        <v>5159000000</v>
       </c>
       <c r="E77">
-        <v>457000000</v>
+        <v>2605000000</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2952,16 +2940,16 @@
         <v>119</v>
       </c>
       <c r="B78">
-        <v>1719000000</v>
+        <v>3273000000</v>
       </c>
       <c r="C78">
-        <v>2430000000</v>
+        <v>2058000000</v>
       </c>
       <c r="D78">
-        <v>791000000</v>
+        <v>2263000000</v>
       </c>
       <c r="E78">
-        <v>632000000</v>
+        <v>1122000000</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2969,16 +2957,16 @@
         <v>120</v>
       </c>
       <c r="B79">
-        <v>9999000000</v>
+        <v>3399000000</v>
       </c>
       <c r="C79">
-        <v>3827000000</v>
+        <v>1505000000</v>
       </c>
       <c r="D79">
-        <v>4650000000</v>
+        <v>466000000</v>
       </c>
       <c r="E79">
-        <v>2429000000</v>
+        <v>692000000</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2986,72 +2974,66 @@
         <v>121</v>
       </c>
       <c r="B80">
-        <v>9999000000</v>
+        <v>3408000000</v>
       </c>
       <c r="C80">
-        <v>3827000000</v>
+        <v>1719000000</v>
       </c>
       <c r="D80">
-        <v>4650000000</v>
+        <v>2430000000</v>
       </c>
       <c r="E80">
-        <v>2429000000</v>
+        <v>791000000</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="B81">
+        <v>23065000000</v>
+      </c>
+      <c r="C81">
+        <v>9999000000</v>
+      </c>
+      <c r="D81">
+        <v>3827000000</v>
+      </c>
       <c r="E81">
-        <v>-21000000</v>
-      </c>
-      <c r="F81">
-        <v>-11000000</v>
+        <v>4650000000</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="B82">
+        <v>23065000000</v>
+      </c>
+      <c r="C82">
+        <v>9999000000</v>
+      </c>
+      <c r="D82">
+        <v>3827000000</v>
+      </c>
       <c r="E82">
-        <v>2450000000</v>
-      </c>
-      <c r="F82">
-        <v>1668000000</v>
+        <v>4650000000</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B83">
-        <v>25984000000</v>
-      </c>
-      <c r="C83">
-        <v>13296000000</v>
-      </c>
-      <c r="D83">
-        <v>21208000000</v>
-      </c>
-      <c r="E83">
-        <v>11561000000</v>
+      <c r="F83">
+        <v>-21000000</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B84">
-        <v>18704000000</v>
-      </c>
-      <c r="C84">
-        <v>9907000000</v>
-      </c>
-      <c r="D84">
-        <v>19218000000</v>
-      </c>
-      <c r="E84">
-        <v>10714000000</v>
+      <c r="F84">
+        <v>2450000000</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3059,16 +3041,50 @@
         <v>126</v>
       </c>
       <c r="B85">
+        <v>43210000000</v>
+      </c>
+      <c r="C85">
+        <v>25984000000</v>
+      </c>
+      <c r="D85">
+        <v>13296000000</v>
+      </c>
+      <c r="E85">
+        <v>21208000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B86">
+        <v>34621000000</v>
+      </c>
+      <c r="C86">
+        <v>18704000000</v>
+      </c>
+      <c r="D86">
+        <v>9907000000</v>
+      </c>
+      <c r="E86">
+        <v>19218000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87">
+        <v>8589000000</v>
+      </c>
+      <c r="C87">
         <v>7280000000</v>
       </c>
-      <c r="C85">
+      <c r="D87">
         <v>3389000000</v>
       </c>
-      <c r="D85">
+      <c r="E87">
         <v>1990000000</v>
-      </c>
-      <c r="E85">
-        <v>847000000</v>
       </c>
     </row>
   </sheetData>
@@ -3078,7 +3094,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3086,50 +3102,50 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1">
+        <v>45688</v>
+      </c>
+      <c r="C1" s="1">
         <v>45322</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>44957</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>44592</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>44227</v>
-      </c>
-      <c r="F1" s="1">
-        <v>43861</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B2">
+        <v>60853000000</v>
+      </c>
+      <c r="C2">
         <v>27021000000</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>3808000000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>8132000000</v>
-      </c>
-      <c r="E2">
-        <v>4694000000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B3">
+        <v>-33706000000</v>
+      </c>
+      <c r="C3">
         <v>-9533000000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>-10039000000</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3137,254 +3153,254 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4">
         <v>-1250000000</v>
       </c>
       <c r="C4">
+        <v>-1250000000</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-1000000000</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>4977000000</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>4968000000</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B6">
+        <v>-3236000000</v>
+      </c>
+      <c r="C6">
         <v>-1069000000</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-1833000000</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-976000000</v>
-      </c>
-      <c r="E6">
-        <v>-1128000000</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B7">
+        <v>246000000</v>
+      </c>
+      <c r="C7">
         <v>252000000</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>254000000</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>246000000</v>
-      </c>
-      <c r="E7">
-        <v>138000000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B8">
+        <v>15118000000</v>
+      </c>
+      <c r="C8">
         <v>6549000000</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1404000000</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>396000000</v>
-      </c>
-      <c r="E8">
-        <v>249000000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B9">
+        <v>8589000000</v>
+      </c>
+      <c r="C9">
         <v>7280000000</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>3389000000</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1990000000</v>
-      </c>
-      <c r="E9">
-        <v>847000000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B10">
+        <v>7280000000</v>
+      </c>
+      <c r="C10">
         <v>3389000000</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1990000000</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>847000000</v>
-      </c>
-      <c r="E10">
-        <v>10896000000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B11">
+        <v>1309000000</v>
+      </c>
+      <c r="C11">
         <v>3891000000</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1399000000</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1143000000</v>
-      </c>
-      <c r="E11">
-        <v>-10049000000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B12">
+        <v>-42359000000</v>
+      </c>
+      <c r="C12">
         <v>-13633000000</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>-11617000000</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1865000000</v>
-      </c>
-      <c r="E12">
-        <v>3804000000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B13">
+        <v>-42359000000</v>
+      </c>
+      <c r="C13">
         <v>-13633000000</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>-11617000000</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1865000000</v>
-      </c>
-      <c r="E13">
-        <v>3804000000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B14">
+        <v>-7059000000</v>
+      </c>
+      <c r="C14">
         <v>-2858000000</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>-1535000000</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>-1994000000</v>
-      </c>
-      <c r="E14">
-        <v>-963000000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B15">
+        <v>490000000</v>
+      </c>
+      <c r="C15">
         <v>403000000</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>355000000</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>281000000</v>
-      </c>
-      <c r="E15">
-        <v>194000000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B16">
+        <v>-834000000</v>
+      </c>
+      <c r="C16">
         <v>-395000000</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>-398000000</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>-399000000</v>
-      </c>
-      <c r="E16">
-        <v>-395000000</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
+      </c>
+      <c r="B17">
+        <v>-834000000</v>
       </c>
       <c r="C17">
+        <v>-395000000</v>
+      </c>
+      <c r="D17">
         <v>-398000000</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-399000000</v>
-      </c>
-      <c r="E17">
-        <v>-395000000</v>
-      </c>
-      <c r="F17">
-        <v>-390000000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B18">
+        <v>-33706000000</v>
+      </c>
+      <c r="C18">
         <v>-9533000000</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>-10039000000</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -3392,16 +3408,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B19">
+        <v>-33706000000</v>
+      </c>
+      <c r="C19">
         <v>-9533000000</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>-10039000000</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -3409,610 +3425,658 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B20">
         <v>-1250000000</v>
       </c>
       <c r="C20">
+        <v>-1250000000</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>3977000000</v>
-      </c>
-      <c r="E20">
-        <v>4968000000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B21">
         <v>-1250000000</v>
       </c>
       <c r="C21">
+        <v>-1250000000</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>3977000000</v>
-      </c>
-      <c r="E21">
-        <v>4968000000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B22">
         <v>-1250000000</v>
       </c>
       <c r="C22">
+        <v>-1250000000</v>
+      </c>
+      <c r="D22">
         <v>0</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>-1000000000</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>4977000000</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>4968000000</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B24">
+        <v>-20421000000</v>
+      </c>
+      <c r="C24">
         <v>-10566000000</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>7375000000</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>-9830000000</v>
-      </c>
-      <c r="E24">
-        <v>-19675000000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B25">
+        <v>-20421000000</v>
+      </c>
+      <c r="C25">
         <v>-10566000000</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>7375000000</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>-9830000000</v>
-      </c>
-      <c r="E25">
-        <v>-19675000000</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B26">
-        <v>-9414000000</v>
+        <v>22000000</v>
       </c>
       <c r="C26">
-        <v>9257000000</v>
-      </c>
-      <c r="D26">
-        <v>-8591000000</v>
-      </c>
-      <c r="E26">
-        <v>-10023000000</v>
+        <v>-124000000</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B27">
-        <v>9782000000</v>
+        <v>-16200000000</v>
       </c>
       <c r="C27">
-        <v>21231000000</v>
+        <v>-9290000000</v>
       </c>
       <c r="D27">
-        <v>16220000000</v>
+        <v>9257000000</v>
       </c>
       <c r="E27">
-        <v>9319000000</v>
+        <v>-8591000000</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B28">
-        <v>-19196000000</v>
+        <v>11861000000</v>
       </c>
       <c r="C28">
-        <v>-11974000000</v>
+        <v>9783000000</v>
       </c>
       <c r="D28">
-        <v>-24811000000</v>
+        <v>21239000000</v>
       </c>
       <c r="E28">
-        <v>-19342000000</v>
+        <v>16220000000</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B29">
-        <v>-83000000</v>
+        <v>-28061000000</v>
       </c>
       <c r="C29">
-        <v>-49000000</v>
+        <v>-19073000000</v>
       </c>
       <c r="D29">
-        <v>-263000000</v>
+        <v>-11982000000</v>
       </c>
       <c r="E29">
-        <v>-8524000000</v>
+        <v>-24811000000</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B30">
+        <v>-1007000000</v>
+      </c>
+      <c r="C30">
         <v>-83000000</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>-49000000</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>-263000000</v>
-      </c>
-      <c r="E30">
-        <v>-8524000000</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B31">
-        <v>-1069000000</v>
+        <v>-1007000000</v>
       </c>
       <c r="C31">
-        <v>-1833000000</v>
+        <v>-83000000</v>
       </c>
       <c r="D31">
-        <v>-976000000</v>
+        <v>-49000000</v>
       </c>
       <c r="E31">
-        <v>-1128000000</v>
+        <v>-263000000</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
+        <v>159</v>
+      </c>
+      <c r="B32">
+        <v>-3236000000</v>
+      </c>
+      <c r="C32">
+        <v>-1069000000</v>
+      </c>
+      <c r="D32">
+        <v>-1833000000</v>
+      </c>
+      <c r="E32">
+        <v>-976000000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B33">
+        <v>-3236000000</v>
+      </c>
+      <c r="C33">
         <v>-1069000000</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>-1833000000</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>-976000000</v>
-      </c>
-      <c r="E33">
-        <v>-1128000000</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E34">
+        <v>161</v>
+      </c>
+      <c r="F34">
         <v>-1128000000</v>
-      </c>
-      <c r="F34">
-        <v>-489000000</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B35">
+        <v>64089000000</v>
+      </c>
+      <c r="C35">
         <v>28090000000</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>5641000000</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>9108000000</v>
-      </c>
-      <c r="E35">
-        <v>5822000000</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B36">
+        <v>64089000000</v>
+      </c>
+      <c r="C36">
         <v>28090000000</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>5641000000</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>9108000000</v>
-      </c>
-      <c r="E36">
-        <v>5822000000</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B37">
+        <v>-9383000000</v>
+      </c>
+      <c r="C37">
         <v>-3722000000</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>-2207000000</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>-3363000000</v>
-      </c>
-      <c r="E37">
-        <v>-703000000</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38">
+        <v>165</v>
+      </c>
+      <c r="F38">
         <v>163000000</v>
-      </c>
-      <c r="F38">
-        <v>28000000</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B39">
+        <v>1221000000</v>
+      </c>
+      <c r="C39">
         <v>514000000</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>252000000</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>192000000</v>
-      </c>
-      <c r="E39">
-        <v>163000000</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B40">
+        <v>7635000000</v>
+      </c>
+      <c r="C40">
         <v>3556000000</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>790000000</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>1149000000</v>
-      </c>
-      <c r="E40">
-        <v>602000000</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B41">
+        <v>4278000000</v>
+      </c>
+      <c r="C41">
         <v>2025000000</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>1341000000</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>581000000</v>
-      </c>
-      <c r="E41">
-        <v>290000000</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B42">
+        <v>3357000000</v>
+      </c>
+      <c r="C42">
         <v>1531000000</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>-551000000</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>568000000</v>
-      </c>
-      <c r="E42">
-        <v>312000000</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B43">
+        <v>3357000000</v>
+      </c>
+      <c r="C43">
         <v>1531000000</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>-551000000</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>568000000</v>
-      </c>
-      <c r="E43">
-        <v>312000000</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B44">
+        <v>-395000000</v>
+      </c>
+      <c r="C44">
         <v>-1522000000</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>-1517000000</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>-1715000000</v>
-      </c>
-      <c r="E44">
-        <v>-394000000</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B45">
+        <v>-4781000000</v>
+      </c>
+      <c r="C45">
         <v>-98000000</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>-2554000000</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>-774000000</v>
-      </c>
-      <c r="E45">
-        <v>-524000000</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B46">
+        <v>-13063000000</v>
+      </c>
+      <c r="C46">
         <v>-6172000000</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>822000000</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>-2215000000</v>
-      </c>
-      <c r="E46">
-        <v>-550000000</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B47">
+        <v>-13063000000</v>
+      </c>
+      <c r="C47">
         <v>-6172000000</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>822000000</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>-2215000000</v>
-      </c>
-      <c r="E47">
-        <v>-550000000</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B48">
+        <v>-502000000</v>
+      </c>
+      <c r="C48">
         <v>-278000000</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>1346000000</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>47000000</v>
-      </c>
-      <c r="E48">
-        <v>-20000000</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B49">
+        <v>4737000000</v>
+      </c>
+      <c r="C49">
         <v>3549000000</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>2709000000</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>2004000000</v>
-      </c>
-      <c r="E49">
-        <v>1397000000</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B50">
+        <v>-4477000000</v>
+      </c>
+      <c r="C50">
         <v>-2489000000</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>-2164000000</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>-406000000</v>
-      </c>
-      <c r="E50">
-        <v>-282000000</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B51">
+        <v>-4477000000</v>
+      </c>
+      <c r="C51">
         <v>-2489000000</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>-2164000000</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>-406000000</v>
-      </c>
-      <c r="E51">
-        <v>-282000000</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B52">
+        <v>1864000000</v>
+      </c>
+      <c r="C52">
         <v>1508000000</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>1544000000</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>1174000000</v>
-      </c>
-      <c r="E52">
-        <v>1098000000</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B53">
+        <v>1864000000</v>
+      </c>
+      <c r="C53">
         <v>1508000000</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>1544000000</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>1174000000</v>
-      </c>
-      <c r="E53">
-        <v>1098000000</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B54">
-        <v>-238000000</v>
+        <v>181</v>
       </c>
       <c r="C54">
-        <v>45000000</v>
+        <v>614000000</v>
       </c>
       <c r="D54">
-        <v>-100000000</v>
+        <v>699000000</v>
+      </c>
+      <c r="E54">
+        <v>563000000</v>
       </c>
       <c r="F54">
-        <v>1000000</v>
+        <v>612000000</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B55">
-        <v>-238000000</v>
+        <v>182</v>
       </c>
       <c r="C55">
-        <v>45000000</v>
+        <v>614000000</v>
       </c>
       <c r="D55">
-        <v>-100000000</v>
+        <v>699000000</v>
+      </c>
+      <c r="E55">
+        <v>563000000</v>
       </c>
       <c r="F55">
-        <v>1000000</v>
+        <v>612000000</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B56">
+        <v>183</v>
+      </c>
+      <c r="C56">
+        <v>894000000</v>
+      </c>
+      <c r="D56">
+        <v>844000000</v>
+      </c>
+      <c r="E56">
+        <v>611000000</v>
+      </c>
+      <c r="F56">
+        <v>486000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57">
+        <v>-1030000000</v>
+      </c>
+      <c r="C57">
+        <v>-238000000</v>
+      </c>
+      <c r="D57">
+        <v>45000000</v>
+      </c>
+      <c r="E57">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58">
+        <v>-1030000000</v>
+      </c>
+      <c r="C58">
+        <v>-238000000</v>
+      </c>
+      <c r="D58">
+        <v>45000000</v>
+      </c>
+      <c r="E58">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59">
+        <v>72880000000</v>
+      </c>
+      <c r="C59">
         <v>29760000000</v>
       </c>
-      <c r="C56">
+      <c r="D59">
         <v>4368000000</v>
       </c>
-      <c r="D56">
+      <c r="E59">
         <v>9752000000</v>
-      </c>
-      <c r="E56">
-        <v>4332000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>